<commit_message>
add find multi url
</commit_message>
<xml_diff>
--- a/responses/business-standard.com.xlsx
+++ b/responses/business-standard.com.xlsx
@@ -477,27 +477,27 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nostalgia, gravitas and credibility: How brand Bachchan stands tall at 80s - Business Standard</t>
+          <t>Indiana Supreme Court puts state Republican-backed abortion ban on hold - Business Standard</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/nostalgia-gravitas-and-credibility-how-brand-bachchan-stands-tall-at-80-122101101428_1.html</t>
+          <t>https://www.business-standard.com/article/international/indiana-supreme-court-puts-state-republican-backed-abortion-ban-on-hold-122101300052_1.html</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CAIiEIa54hoYZtNFNZoPJgVwx9YqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEI1Ohp3-fXOzgAxDjMeqThwqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:09:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:59:00 GMT</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Nostalgia, gravitas and credibility: How brand Bachchan stands tall at 80s  Business Standard</t>
+          <t>Indiana Supreme Court puts state Republican-backed abortion ban on hold  Business Standard</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -513,27 +513,27 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mulayam Singh cremated in Saifai, people pay respects in large numberss - Business Standard</t>
+          <t>US in decisive decade in competition with China: NSA Jake Sullivan - Business Standard</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/samajwadi-party-patriarch-mulayam-singh-yadav-cremated-in-saifai-122101100787_1.html</t>
+          <t>https://www.business-standard.com/article/international/us-in-decisive-decade-in-competition-with-china-nsa-jake-sullivan-122101300024_1.html</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CAIiEIYoLMB2xhu_Na85W6Mh1NkqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiEFAPwjdAlRUqRObz0h13MrIqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 11:05:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:36:00 GMT</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Mulayam Singh cremated in Saifai, people pay respects in large numberss  Business Standard</t>
+          <t>US in decisive decade in competition with China: NSA Jake Sullivan  Business Standard</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -549,27 +549,27 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>King Charles coronation to take place on May 6 next year: Buckingham Palaces - Business Standard</t>
+          <t>Latest LIVE: Indias UPI system logistical marvel, says IMF deputy director - Business Standard</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/king-charles-coronation-to-take-place-on-may-6-next-year-buckingham-palace-122101101393_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/latest-news-live-updates-hijab-case-vande-bharat-express-narendra-modi-supreme-court-pmgsy-3-122101300104_1.html</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CAIiEAZZUhsUdIIMpXhSd2_U8l0qGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEB5fuJymy2SK9CJm3sNzZUwqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:31:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:38:00 GMT</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>King Charles coronation to take place on May 6 next year: Buckingham Palaces  Business Standard</t>
+          <t>Latest LIVE: Indias UPI system logistical marvel, says IMF deputy director  Business Standard</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -585,27 +585,27 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IMF cuts Indias FY23 GDP forecast to 6.8%, flags global inflation crisiss - Business Standard</t>
+          <t>Yellen says US economy resilient amid global headwinds; pledges vigilance - Business Standard</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/imf-cuts-india-s-fy23-gdp-growth-forecast-by-60-bps-to-6-8-122101101004_1.html</t>
+          <t>https://www.business-standard.com/article/international/yellen-says-us-economy-resilient-amid-global-headwinds-pledges-vigilance-122101300072_1.html</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CAIiEPgaWvujqENyV0j4rT-9m5wqGQgEKhAIACoHCAowsLXdCjCm3dEBMNPjpAM</t>
+          <t>CAIiEFHfphp8RWT640B5VsDqnxsqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:03:00 GMT</t>
+          <t>Thu, 13 Oct 2022 02:07:00 GMT</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>IMF cuts Indias FY23 GDP forecast to 6.8%, flags global inflation crisiss  Business Standard</t>
+          <t>Yellen says US economy resilient amid global headwinds; pledges vigilance  Business Standard</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -621,27 +621,27 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gujarats Modhera village basks in the sun, awaits solar power benefitss - Business Standard</t>
+          <t>Imran Khan claims someone else pulled strings of power during his tenure - Business Standard</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/gujarat-s-modhera-village-basks-in-the-sun-awaits-solar-power-benefits-122101101326_1.html</t>
+          <t>https://www.business-standard.com/article/international/imran-khan-claims-someone-else-pulled-strings-of-power-during-his-tenure-122101201316_1.html</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CAIiEK7eC-okBDfMP_O3uuk7t4sqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEAGccuqdGYnZ6pt1Y28uBPQqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:32:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:04:00 GMT</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Gujarats Modhera village basks in the sun, awaits solar power benefitss  Business Standard</t>
+          <t>Imran Khan claims someone else pulled strings of power during his tenure  Business Standard</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -657,27 +657,27 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A troubled world: IMF paints a bleak picture - Business Standard</t>
+          <t>Recession fears mount as UK GDP falls 0.3% in Aug after 0.1% growth in July - Business Standard</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/opinion/a-troubled-world-imf-paints-a-bleak-picture-122101101333_1.html</t>
+          <t>https://www.business-standard.com/article/international/recession-fears-mount-as-uk-gdp-falls-0-3-in-aug-after-0-1-growth-in-july-122101300066_1.html</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CAIiEBXhJv1dXZ_UEGEhtREueTAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEH-OOt4G3cBrfyeOEfEfeX8qGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:33:00 GMT</t>
+          <t>Thu, 13 Oct 2022 02:06:00 GMT</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A troubled world: IMF paints a bleak picture  Business Standard</t>
+          <t>Recession fears mount as UK GDP falls 0.3% in Aug after 0.1% growth in July  Business Standard</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -693,27 +693,27 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>It has origins in Maha: Shinde hails Two Swords and Shield poll symbols - Business Standard</t>
+          <t>UN principles must be upheld: India after abstaining on UNGA vote on Russia - Business Standard</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/politics/shinde-hails-two-swords-shield-symbol-says-it-has-origins-in-maha-ld-122101101129_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/un-principles-must-be-upheld-india-after-abstaining-on-unga-vote-on-russia-122101300051_1.html</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CAIiEPIM-1PerDDBIFcttPqOFYUqGQgEKhAIACoHCAowsLXdCjCm3dEBMPPjpAM</t>
+          <t>CBMimAFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jdXJyZW50LWFmZmFpcnMvdW4tcHJpbmNpcGxlcy1tdXN0LWJlLXVwaGVsZC1pbmRpYS1hZnRlci1hYnN0YWluaW5nLW9uLXVuZ2Etdm90ZS1vbi1ydXNzaWEtMTIyMTAxMzAwMDUxXzEuaHRtbNIBnAFodHRwczovL3dhcC5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS1hbXAvY3VycmVudC1hZmZhaXJzL3VuLXByaW5jaXBsZXMtbXVzdC1iZS11cGhlbGQtaW5kaWEtYWZ0ZXItYWJzdGFpbmluZy1vbi11bmdhLXZvdGUtb24tcnVzc2lhLTEyMjEwMTMwMDA1MV8xLmh0bWw</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:31:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:51:00 GMT</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>It has origins in Maha: Shinde hails Two Swords and Shield poll symbols  Business Standard</t>
+          <t>UN principles must be upheld: India after abstaining on UNGA vote on Russia  Business Standard</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -729,27 +729,27 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Targeting infrastructure and causing civilian deaths not acceptable: EAMs - Business Standard</t>
+          <t>Maharashtra govt transfers 20 IAS officers including education commissioner - Business Standard</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/targeting-infrastructure-and-causing-civilian-deaths-not-acceptable-eam-122101100911_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/maharashtra-govt-transfers-20-ias-officers-including-education-commissioner-122101300015_1.html</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CBMilQFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jdXJyZW50LWFmZmFpcnMvdGFyZ2V0aW5nLWluZnJhc3RydWN0dXJlLWFuZC1jYXVzaW5nLWNpdmlsaWFuLWRlYXRocy1ub3QtYWNjZXB0YWJsZS1lYW0tMTIyMTAxMTAwOTExXzEuaHRtbNIBAA</t>
+          <t>CAIiENT7QrfNhQ0z117E7h5FWqMqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:38:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:29:00 GMT</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Targeting infrastructure and causing civilian deaths not acceptable: EAMs  Business Standard</t>
+          <t>Maharashtra govt transfers 20 IAS officers including education commissioner  Business Standard</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -765,27 +765,27 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Israel and Lebanon reach historic deal on gas fields, says reports - Business Standard</t>
+          <t>West Indies tour of Pakistan in 2023 likely to be postponed: Report - Business Standard</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/israel-and-lebanon-reach-historic-deal-on-gas-fields-says-report-122101101349_1.html</t>
+          <t>https://www.business-standard.com/article/sports/west-indies-tour-of-pakistan-in-2023-likely-to-be-postponed-report-122101201397_1.html</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CAIiELDZNJFnnpeM0Erzz7C6phsqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiED986ycZLiq69XiS5uVHWGAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:18:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:18:00 GMT</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Israel and Lebanon reach historic deal on gas fields, says reports  Business Standard</t>
+          <t>West Indies tour of Pakistan in 2023 likely to be postponed: Report  Business Standard</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -801,27 +801,27 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Current account imbalance hits India harder than EM peers, shows datas - Business Standard</t>
+          <t>Centre allows exports of 397,267 tonnes broken rice backed by LoC - Business Standard</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/global-current-account-imbalance-hits-india-worse-than-peers-shows-data-122101101107_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/govt-allows-broken-rice-exports-backed-by-already-issued-letters-of-credit-122101201392_1.html</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CAIiENKwysenEQr_XXy6fVS8MDEqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEM2llTrnw9eBgeU83oDZ3X0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:45:00 GMT</t>
+          <t>Thu, 13 Oct 2022 01:09:00 GMT</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Current account imbalance hits India harder than EM peers, shows datas  Business Standard</t>
+          <t>Centre allows exports of 397,267 tonnes broken rice backed by LoC  Business Standard</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -837,27 +837,27 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mahakal Lok opening: PM Modi unveils shivaling wrapped in sacred threads - Business Standard</t>
+          <t>Fed officials commit to restrictive rates but calibration needed: Minutes - Business Standard</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/pm-modi-inaugurates-mahakal-lok-corridor-at-mahakaleshwar-temple-122101101125_1.html</t>
+          <t>https://www.business-standard.com/article/international/fed-officials-commit-to-restrictive-rates-but-calibration-needed-minutes-122101201386_1.html</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CAIiEMdmiLvwscuKjuxxvxhK-Y4qGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiECDTTrMGbJks0JBoA6TyVOsqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:22:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:08:00 GMT</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Mahakal Lok opening: PM Modi unveils shivaling wrapped in sacred threads  Business Standard</t>
+          <t>Fed officials commit to restrictive rates but calibration needed: Minutes  Business Standard</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -873,27 +873,27 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Spinners shine as India clinches ODI series against South Africas - Business Standard</t>
+          <t>OPEC slashes 2022, 2023 oil demand growth view as economy slows - Business Standard</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/sports/india-beat-south-africa-by-seven-wickets-in-third-odi-to-seal-series-122101101017_1.html</t>
+          <t>https://www.business-standard.com/article/international/opec-slashes-2022-2023-oil-demand-growth-view-as-economy-slows-122101201176_1.html</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CAIiEAQ61vmEcU8niBmOQJpT7MoqGQgEKhAIACoHCAowsLXdCjCm3dEBMMa4swY</t>
+          <t>CAIiEOwrE0kzk-H1R4TKXdB9pZMqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:42:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:52:00 GMT</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Spinners shine as India clinches ODI series against South Africas  Business Standard</t>
+          <t>OPEC slashes 2022, 2023 oil demand growth view as economy slows  Business Standard</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -909,27 +909,27 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>US-China chip war wipes out $240 billion as stocks plunge; TSMC slips 8.3%s - Business Standard</t>
+          <t>Injured Chahar ruled out; Siraj, Shami, Shardul set to join team for T20 WC - Business Standard</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/us-china-chip-war-wipes-out-240-billion-as-stocks-plunge-tsmc-slips-8-3-122101101403_1.html</t>
+          <t>https://www.business-standard.com/article/sports/injured-chahar-ruled-out-siraj-shami-shardul-set-to-join-team-for-t20-wc-122101201074_1.html</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CAIiEN40NY2T-VIKJFHFKtwSMFsqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEHv9dzO1I9N69PLQCSiLEwgqGQgEKhAIACoHCAowsLXdCjCm3dEBMMa4swY</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:26:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:11:00 GMT</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>US-China chip war wipes out $240 billion as stocks plunge; TSMC slips 8.3%s  Business Standard</t>
+          <t>Injured Chahar ruled out; Siraj, Shami, Shardul set to join team for T20 WC  Business Standard</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -945,27 +945,27 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gabbard to leave Democratic Party, calls it elitist cabal of war mongerss - Business Standard</t>
+          <t>Oil down on strong dollar, worries about recession and hawkish Fed talk - Business Standard</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/gabbard-to-leave-democratic-party-calls-it-elitist-cabal-of-war-mongers-122101101328_1.html</t>
+          <t>https://www.business-standard.com/article/international/oil-down-on-strong-dollar-worries-about-recession-and-hawkish-fed-talk-122101201275_1.html</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CAIiEELnBPGYBy7Nwxc1hbb24aUqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEANlVGwlF0J6Ux9Vc6qF9joqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:56:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:01:00 GMT</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Gabbard to leave Democratic Party, calls it elitist cabal of war mongerss  Business Standard</t>
+          <t>Oil down on strong dollar, worries about recession and hawkish Fed talk  Business Standard</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -981,27 +981,27 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>New highly infectious Covid variants emerge in China, says reports - Business Standard</t>
+          <t>Tharoor hails Congress decision to have secret ballot for party prez polls - Business Standard</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/new-highly-infectious-covid-variants-emerge-in-china-says-report-122101101405_1.html</t>
+          <t>https://www.business-standard.com/article/politics/tharoor-hails-congress-decision-to-have-secret-ballot-for-party-prez-polls-122101201249_1.html</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CAIiEC8z3418kgZjCv2vfMn8Pm4qGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEMabsWeTObpVA35Dx1FQ81MqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:42:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:34:00 GMT</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>New highly infectious Covid variants emerge in China, says reports  Business Standard</t>
+          <t>Tharoor hails Congress decision to have secret ballot for party prez polls  Business Standard</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1017,27 +1017,27 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>JPMorgan CEO Jamie Dimon expects US recession in six to nine monthss - Business Standard</t>
+          <t>Microsoft, Meta announce partnership to deliver immersive experiences in VR - Business Standard</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/jpmorgan-ceo-jamie-dimon-expects-us-recession-in-six-to-nine-months-122101101406_1.html</t>
+          <t>https://www.business-standard.com/article/international/microsoft-meta-announce-partnership-to-deliver-immersive-experiences-in-vr-122101200826_1.html</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>CAIiEBKSuvvIquY1Da5qUH1p5EgqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEFfK7-PZkuqfze0W2Q61DRsqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:32:00 GMT</t>
+          <t>Wed, 12 Oct 2022 13:32:00 GMT</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>JPMorgan CEO Jamie Dimon expects US recession in six to nine monthss  Business Standard</t>
+          <t>Microsoft, Meta announce partnership to deliver immersive experiences in VR  Business Standard</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1053,27 +1053,27 @@
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Uber, Lyft slump as US proposal on workers a potential blow to gig economys - Business Standard</t>
+          <t>Wipros secret of reducing attrition: Quarterly promotions, salary hikes - Business Standard</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/uber-lyft-slump-as-us-proposal-on-workers-a-potential-blow-to-gig-economy-122101101344_1.html</t>
+          <t>https://www.business-standard.com/article/companies/wipro-s-secret-of-reducing-attrition-promotions-and-salary-hikes-122101201154_1.html</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CAIiEAdW8_OUwY8JNG0wSguyMNQqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CBMiiAFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jb21wYW5pZXMvd2lwcm8tcy1zZWNyZXQtb2YtcmVkdWNpbmctYXR0cml0aW9uLXByb21vdGlvbnMtYW5kLXNhbGFyeS1oaWtlcy0xMjIxMDEyMDExNTRfMS5odG1s0gGMAWh0dHBzOi8vd2FwLmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlLWFtcC9jb21wYW5pZXMvd2lwcm8tcy1zZWNyZXQtb2YtcmVkdWNpbmctYXR0cml0aW9uLXByb21vdGlvbnMtYW5kLXNhbGFyeS1oaWtlcy0xMjIxMDEyMDExNTRfMS5odG1s</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:06:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:05:00 GMT</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Uber, Lyft slump as US proposal on workers a potential blow to gig economys  Business Standard</t>
+          <t>Wipros secret of reducing attrition: Quarterly promotions, salary hikes  Business Standard</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1089,27 +1089,27 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>T20 WC: INOX signs deal with ICC to live screen India matches in cinemass - Business Standard</t>
+          <t>5G services to go live on Samsung devices, iPhones in November-December - Business Standard</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/t20-wc-inox-signs-deal-with-icc-to-live-screen-india-matches-in-cinemas-122101101111_1.html</t>
+          <t>https://www.business-standard.com/article/companies/samsung-5g-smartphones-likely-to-get-software-support-by-mid-november-122101200976_1.html</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CAIiEBGQ_iwztNtq0xGnsjxhx4AqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEBrg3CrI14Nh5eSisS-jWJsqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:34:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:32:00 GMT</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>T20 WC: INOX signs deal with ICC to live screen India matches in cinemass  Business Standard</t>
+          <t>5G services to go live on Samsung devices, iPhones in November-December  Business Standard</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1125,27 +1125,27 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Markets fall most in 2 weeks on rising yields; Sensex declines 844 pointss - Business Standard</t>
+          <t>Microsoft unveils Surface devices, Apple services integration in Windows 11 - Business Standard</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/markets/sensex-nifty-drop-over-1-amid-rising-yields-geopolitical-concerns-122101101022_1.html</t>
+          <t>https://www.business-standard.com/article/technology/microsoft-unveils-surface-devices-apple-services-integration-in-windows-11-122101201171_1.html</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>CBMihwFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9tYXJrZXRzL3NlbnNleC1uaWZ0eS1kcm9wLW92ZXItMS1hbWlkLXJpc2luZy15aWVsZHMtZ2VvcG9saXRpY2FsLWNvbmNlcm5zLTEyMjEwMTEwMTAyMl8xLmh0bWzSAQA</t>
+          <t>CAIiEHMHnEOhGbF8lK-bT773p7sqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:39:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:50:00 GMT</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Markets fall most in 2 weeks on rising yields; Sensex declines 844 pointss  Business Standard</t>
+          <t>Microsoft unveils Surface devices, Apple services integration in Windows 11  Business Standard</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1161,27 +1161,27 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>How are Employee Assistance Programs making a difference in corporate wellness? - Business Standard</t>
+          <t>Nitish slams Amit Shah, says he has no knowledge of our countrys history - Business Standard</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/content/specials/how-are-employee-assistance-programs-making-a-difference-in-corporate-wellness-122101200021_1.html</t>
+          <t>https://www.business-standard.com/article/politics/nitish-slams-amit-shah-says-he-has-no-knowledge-of-our-country-s-history-122101201227_1.html</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>CBMilQFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vY29udGVudC9zcGVjaWFscy9ob3ctYXJlLWVtcGxveWVlLWFzc2lzdGFuY2UtcHJvZ3JhbXMtbWFraW5nLWEtZGlmZmVyZW5jZS1pbi1jb3Jwb3JhdGUtd2VsbG5lc3MtMTIyMTAxMjAwMDIxXzEuaHRtbNIBAA</t>
+          <t>CAIiEMkx1-c2r83q8BRnp5-smngqGQgEKhAIACoHCAowsLXdCjCm3dEBMPPjpAM</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 19:26:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:14:00 GMT</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>How are Employee Assistance Programs making a difference in corporate wellness?  Business Standard</t>
+          <t>Nitish slams Amit Shah, says he has no knowledge of our countrys history  Business Standard</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1197,27 +1197,27 @@
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Jio 5G network records top median speed of 600 mbps, beats Airtel: Ooklas - Business Standard</t>
+          <t>Drug regulator halts production at Maiden Pharmas Sonipat unit - Business Standard</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/jio-5g-network-records-top-median-speed-of-600-mbps-beats-airtel-ookla-122101101301_1.html</t>
+          <t>https://www.business-standard.com/article/companies/indian-drug-regulator-halts-production-at-maiden-pharma-sonipat-plant-122101201062_1.html</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>CAIiEPMTCVCF_tXyEscEOkBaCesqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiECFPiIVHYT-iwWyi-J6dOhYqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:23:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:57:00 GMT</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Jio 5G network records top median speed of 600 mbps, beats Airtel: Ooklas  Business Standard</t>
+          <t>Drug regulator halts production at Maiden Pharmas Sonipat unit  Business Standard</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1233,27 +1233,27 @@
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PM Gati Shakti: 197 critical infra gap projects identified in last one years - Business Standard</t>
+          <t>PKL 9: Maninder Singh shines as Bengal Warriors thrash Bengaluru Bulls - Business Standard</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/pm-gatishakti-197-critical-infra-gap-projects-identified-in-last-one-year-122101101189_1.html</t>
+          <t>https://www.business-standard.com/article/sports/pkl-9-maninder-singh-shines-as-bengal-warriors-thrash-bengaluru-bulls-122101201345_1.html</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>CAIiEOhrXR4Ea9H22nAgcuVq0wUqGQgEKhAIACoHCAowsLXdCjCm3dEBMNPjpAM</t>
+          <t>CAIiEC8d2oec2b4SZSqnwk-QbsAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 19:13:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:00:00 GMT</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>PM Gati Shakti: 197 critical infra gap projects identified in last one years  Business Standard</t>
+          <t>PKL 9: Maninder Singh shines as Bengal Warriors thrash Bengaluru Bulls  Business Standard</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1269,27 +1269,27 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>IndiGo to operate wide body planes for first time ever in next few monthss - Business Standard</t>
+          <t>US dollar surges to new 24-year high versus yen; sterling rallies - Business Standard</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/indigo-to-operate-wide-body-planes-for-first-time-ever-in-next-few-months-122101200008_1.html</t>
+          <t>https://www.business-standard.com/article/international/us-dollar-surges-to-new-24-year-high-versus-yen-sterling-rallies-122101201200_1.html</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CAIiELSNKi8BeHFMlKv3hrYsz6gqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiELqWNKw71kQBuvblthHc9mwqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:51:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:16:00 GMT</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>IndiGo to operate wide body planes for first time ever in next few monthss  Business Standard</t>
+          <t>US dollar surges to new 24-year high versus yen; sterling rallies  Business Standard</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1305,27 +1305,27 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tracxn Technologies IPO bought 53% on second day of the issues - Business Standard</t>
+          <t>Disapprove moonlighting, but issue not a big problem in company: HCL Tech - Business Standard</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/markets/tracxn-technologies-ipo-bought-53-on-second-day-of-the-issue-122101101413_1.html</t>
+          <t>https://www.business-standard.com/article/companies/disapprove-moonlighting-but-issue-not-a-big-problem-in-company-hcl-tech-122101201299_1.html</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CAIiEMAkhvEtpKEheJcsSdkpvwIqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEJzsS4cK_M1KodXQE5zjOukqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:43:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:51:00 GMT</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Tracxn Technologies IPO bought 53% on second day of the issues  Business Standard</t>
+          <t>Disapprove moonlighting, but issue not a big problem in company: HCL Tech  Business Standard</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1341,27 +1341,27 @@
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RBI asks banks to set aside capital, provisions for unhedged FX exposures - Business Standard</t>
+          <t>Sensex and Nifty rebound nearly 1%, snap three-day losing run - Business Standard</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/finance/rbi-says-bks-have-to-set-aside-capital-provisions-for-unhedged-fx-exposure-122101101218_1.html</t>
+          <t>https://www.business-standard.com/article/markets/sensex-and-nifty-rebound-nearly-1-snap-three-day-losing-run-122101201313_1.html</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>CBMikAFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9maW5hbmNlL3JiaS1zYXlzLWJrcy1oYXZlLXRvLXNldC1hc2lkZS1jYXBpdGFsLXByb3Zpc2lvbnMtZm9yLXVuaGVkZ2VkLWZ4LWV4cG9zdXJlLTEyMjEwMTEwMTIxOF8xLmh0bWzSAQA</t>
+          <t>CAIiENz_C700uRddExZLCD9GdjcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:07:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:41:00 GMT</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>RBI asks banks to set aside capital, provisions for unhedged FX exposures  Business Standard</t>
+          <t>Sensex and Nifty rebound nearly 1%, snap three-day losing run  Business Standard</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1377,27 +1377,27 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Credit Suisse faces US tax probe, Senate inquiry over accounts: Reports - Business Standard</t>
+          <t>India macro indicators may return to FY20 levels by FY27, says IMF - Business Standard</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/credit-suisse-faces-us-tax-probe-senate-inquiry-over-accounts-report-122101101418_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/india-s-macro-indicators-to-remain-above-pre-pandemic-level-imf-122101200986_1.html</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>CAIiEJMb4XTHMyTvVhvkz4iTgH8qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEDmzJoZE8C_mV80e7rUh1REqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:54:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:34:05 GMT</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Credit Suisse faces US tax probe, Senate inquiry over accounts: Reports  Business Standard</t>
+          <t>India macro indicators may return to FY20 levels by FY27, says IMF  Business Standard</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1413,27 +1413,27 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Karnataka govt orders Ola, Uber, Rapido to stop auto services from Oct 12s - Business Standard</t>
+          <t>PepsiCos beverage volume logs double-digit growth in September quarter - Business Standard</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/karnataka-govt-orders-ola-uber-rapido-to-stop-auto-services-from-oct-12-122101101432_1.html</t>
+          <t>https://www.business-standard.com/article/companies/pepsico-s-beverage-volume-logs-double-digit-growth-in-september-quarter-122101201366_1.html</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>CAIiELZt0Gwuat4XTgpwXYodlKcqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiEO7Z1F6T2K9APhsn42Z7idIqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:10:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:37:00 GMT</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Karnataka govt orders Ola, Uber, Rapido to stop auto services from Oct 12s  Business Standard</t>
+          <t>PepsiCos beverage volume logs double-digit growth in September quarter  Business Standard</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1449,27 +1449,27 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cathie Woods ARKK on the verge of taking out its Covid-19 lows - Business Standard</t>
+          <t>No citizen can be prosecuted under Section 66A IT Act: Supreme Court - Business Standard</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/cathie-wood-s-arkk-on-the-verge-of-taking-out-its-covid-19-low-122101101400_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/supreme-court-issues-guidelines-to-implement-shreya-singhal-s-judgement-122101200937_1.html</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>CAIiEHQjQoaYYHa144qeATYYChkqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEBZqVUyUDcxo4RhAO5hKBRkqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:24:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:10:00 GMT</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Cathie Woods ARKK on the verge of taking out its Covid-19 lows  Business Standard</t>
+          <t>No citizen can be prosecuted under Section 66A IT Act: Supreme Court  Business Standard</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1485,27 +1485,27 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>October rains 80% more than normal over the country; North India leadss - Business Standard</t>
+          <t>Kerala human sacrifice case: Prime accused labelled a psychopath, pervert - Business Standard</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/october-rains-80-more-than-normal-over-the-country-north-india-leads-122101101074_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/kerala-human-sacrifice-case-prime-accused-labelled-a-psychopath-pervert-122101200665_1.html</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CBMikQFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9lY29ub215LXBvbGljeS9vY3RvYmVyLXJhaW5zLTgwLW1vcmUtdGhhbi1ub3JtYWwtb3Zlci10aGUtY291bnRyeS1ub3J0aC1pbmRpYS1sZWFkcy0xMjIxMDExMDEwNzRfMS5odG1s0gEA</t>
+          <t>CAIiEND5bzbkvDLQyhQp1jAfeu0qGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:19:00 GMT</t>
+          <t>Wed, 12 Oct 2022 13:50:00 GMT</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>October rains 80% more than normal over the country; North India leadss  Business Standard</t>
+          <t>Kerala human sacrifice case: Prime accused labelled a psychopath, pervert  Business Standard</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1521,27 +1521,27 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Land lease continuity for Rail landholders, more clarity for Concor sales - Business Standard</t>
+          <t>MP minister slams Aamir Khan for hurting sentiments in bank advertisement - Business Standard</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/land-lease-continuity-for-rail-landholders-more-clarity-for-concor-sale-122101100779_1.html</t>
+          <t>https://www.business-standard.com/article/pti-stories/aamir-khan-should-not-hurt-religious-sentiments-mp-home-minister-on-ad-featuring-actor-122101200650_1.html</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>CAIiENcJvAhSsSLclgjsVr7l26sqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEDAn6225GQ1lRXeuC5QJTHYqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:15:18 GMT</t>
+          <t>Wed, 12 Oct 2022 17:46:00 GMT</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Land lease continuity for Rail landholders, more clarity for Concor sales  Business Standard</t>
+          <t>MP minister slams Aamir Khan for hurting sentiments in bank advertisement  Business Standard</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1557,27 +1557,27 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Start-up EV makers allege partial treatment, halt of FAME subsidies - Business Standard</t>
+          <t>Ukrainian forces recaptures 5 settlements in southern Kherson region - Business Standard</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/start-ups-allege-partial-treatment-halt-of-fame-ii-scheme-subsidies-122101100894_1.html</t>
+          <t>https://www.business-standard.com/article/international/ukrainian-forces-recaptures-5-settlements-in-southern-kherson-region-122101200529_1.html</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>CAIiEFZLs3IJBnVz4SfPM1W3T6QqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEOYTD1gp7X3wwuy1FmMrmiMqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:12:00 GMT</t>
+          <t>Wed, 12 Oct 2022 08:35:00 GMT</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Start-up EV makers allege partial treatment, halt of FAME subsidies  Business Standard</t>
+          <t>Ukrainian forces recaptures 5 settlements in southern Kherson region  Business Standard</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1593,27 +1593,27 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Delhi gets 128.2 mm rain this month, highest for October since 1956s - Business Standard</t>
+          <t>Global wealth set to contract by over 2% this year, says report - Business Standard</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/delhi-gets-128-2-mm-rain-this-month-highest-for-october-since-1956-122101101194_1.html</t>
+          <t>https://www.business-standard.com/article/international/global-wealth-set-to-contract-by-over-2-this-year-says-report-122101201388_1.html</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>CAIiEE6VA-cmShSF1gCRwL0rgksqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEDHc002f6bL9M1qDqecbMQ8qGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:08:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:13:00 GMT</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Delhi gets 128.2 mm rain this month, highest for October since 1956s  Business Standard</t>
+          <t>Global wealth set to contract by over 2% this year, says report  Business Standard</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1629,27 +1629,27 @@
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>UNGA: India votes with West on 3 procedural matters, silent on Ukraines - Business Standard</t>
+          <t>DU issues academic calendar for first semester; classes to begin from Nov 2 - Business Standard</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/unga-india-votes-with-west-on-3-procedural-matters-silent-on-ukraine-122101100319_1.html</t>
+          <t>https://www.business-standard.com/article/education/du-issues-academic-calendar-for-first-semester-classes-to-begin-from-nov-2-122101201252_1.html</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>CAIiELO7u25cKo7h7KUWaCKjT-0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNPjpAM</t>
+          <t>CAIiECippJYr4Ug9sUW5y7Ho5SYqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 06:46:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:27:00 GMT</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>UNGA: India votes with West on 3 procedural matters, silent on Ukraines  Business Standard</t>
+          <t>DU issues academic calendar for first semester; classes to begin from Nov 2  Business Standard</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1665,27 +1665,27 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Start-up funding nosedives by 80% in Q3 and CY22: Tracxn reports - Business Standard</t>
+          <t>Macro policy for uncertain times - Business Standard</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/start-up-funding-nosedives-by-80-in-q3-and-cy22-tracxn-report-122101101425_1.html</t>
+          <t>https://www.business-standard.com/article/opinion/macro-policy-for-uncertain-times-122101201337_1.html</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>CAIiEBqbemXTBmS6GsDfrzmecCwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEIAgvK6PxGHBQqu9zj79q_kqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 18:02:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:01:00 GMT</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Start-up funding nosedives by 80% in Q3 and CY22: Tracxn reports  Business Standard</t>
+          <t>Macro policy for uncertain times  Business Standard</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1701,27 +1701,27 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ravi Kumar S resigns as president effective today, says Infosyss - Business Standard</t>
+          <t>Digital rupee likely to bring down cost of cross-border payments - Business Standard</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/ravi-kumar-s-resigns-as-president-effective-today-says-infosys-122101101334_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/cbdcs-likely-to-lower-cost-of-cross-border-payments-for-the-customers-122101200924_1.html</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>CAIiEGVciVrisr-vRmsfkLYo0KUqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEPMlj6ylKZRHN37PZikMm1sqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:35:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:11:00 GMT</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Ravi Kumar S resigns as president effective today, says Infosyss  Business Standard</t>
+          <t>Digital rupee likely to bring down cost of cross-border payments  Business Standard</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1737,27 +1737,27 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>At least 30 people from Solapur lose money on crypto cloud mining apps - Business Standard</t>
+          <t>Unicorns become cockroaches as tech funding dries up: Report - Business Standard</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/at-least-30-people-from-solapur-lose-money-on-crypto-cloud-mining-app-122101101411_1.html</t>
+          <t>https://www.business-standard.com/article/international/unicorns-become-cockroaches-as-tech-funding-dries-up-report-122101201395_1.html</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>CAIiEFGyYE0rE3auDOn--_Ndj3QqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEIOO_FeBcrhUjvxbqCFVV-AqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:46:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:20:00 GMT</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>At least 30 people from Solapur lose money on crypto cloud mining apps  Business Standard</t>
+          <t>Unicorns become cockroaches as tech funding dries up: Report  Business Standard</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1773,27 +1773,27 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CCTV cams, panic buttons: Features of newly inducted cluster buses in Delhis - Business Standard</t>
+          <t>RBI says regulated bodies cant get fresh ratings from Brickwork Ratings - Business Standard</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/cctv-cams-panic-buttons-features-of-newly-inducted-cluster-buses-in-delhi-122101101306_1.html</t>
+          <t>https://www.business-standard.com/article/companies/rbi-says-regulated-bodies-can-t-get-fresh-ratings-from-brickwork-ratings-122101201102_1.html</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>CAIiEMseuweJchiCbXqQnoDRnvQqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEPTlZyCpF868n1HLs9yjBacqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:54:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:06:00 GMT</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>CCTV cams, panic buttons: Features of newly inducted cluster buses in Delhis  Business Standard</t>
+          <t>RBI says regulated bodies cant get fresh ratings from Brickwork Ratings  Business Standard</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1809,27 +1809,27 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tata Group has no plans to enter 5G consumer space, says N Chandrasekarans - Business Standard</t>
+          <t>CIL will achieve 1 bn tonne coal production target by FY26: Pralhad Joshi - Business Standard</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/tata-group-has-no-plans-to-enter-5g-consumer-space-says-n-chandrasekaran-122101101385_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/cil-will-achieve-1-bn-tonne-coal-production-target-by-fy26-pralhad-joshi-122101201240_1.html</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>CAIiENZy6W1_mFrZvcX31wrinzIqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEADmylg3Js97sJf6sBjywRIqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:35:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:43:00 GMT</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Tata Group has no plans to enter 5G consumer space, says N Chandrasekarans  Business Standard</t>
+          <t>CIL will achieve 1 bn tonne coal production target by FY26: Pralhad Joshi  Business Standard</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1845,27 +1845,27 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MFs see rise in redemption pressure amid spike in inflows across categoriess - Business Standard</t>
+          <t>Retailers likely to see strong revenue performance in July-Sept quarter - Business Standard</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/markets/mfs-see-rise-in-redemption-pressure-amid-spike-in-inflows-across-categories-122101100905_1.html</t>
+          <t>https://www.business-standard.com/article/companies/retailers-likely-to-see-strong-revenue-performance-in-july-sept-quarter-122101201025_1.html</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>CAIiEPBEe-OE8cqH2PHWWBHQl8EqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEKz2fw_WXd4kPkRhvDPfe2YqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:32:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:07:00 GMT</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>MFs see rise in redemption pressure amid spike in inflows across categoriess  Business Standard</t>
+          <t>Retailers likely to see strong revenue performance in July-Sept quarter  Business Standard</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1881,27 +1881,27 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bihar CM after changing sides 5 times: Amit Shah takes a jibe at Nitishs - Business Standard</t>
+          <t>Zoho Corporations business operating system grows 150% in last two years - Business Standard</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/politics/bihar-cm-after-changing-sides-5-times-amit-shah-takes-a-jibe-at-nitish-122101101180_1.html</t>
+          <t>https://www.business-standard.com/article/companies/zoho-corporation-s-business-operating-system-grows-150-in-last-two-years-122101201167_1.html</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>CAIiEA8xo-eEudNdrdYcnUXUqnEqGQgEKhAIACoHCAowsLXdCjCm3dEBMPPjpAM</t>
+          <t>CAIiEObS-ACdG9bLbPJGSwIj97sqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:02:00 GMT</t>
+          <t>Wed, 12 Oct 2022 18:04:00 GMT</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Bihar CM after changing sides 5 times: Amit Shah takes a jibe at Nitishs  Business Standard</t>
+          <t>Zoho Corporations business operating system grows 150% in last two years  Business Standard</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -1917,27 +1917,27 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>IndiGo to launch Mumbai-Istanbul flights from Jan 1, bookings begins - Business Standard</t>
+          <t>Budget focus is to maintain growth, tame inflation: FM Nirmala Sitharaman - Business Standard</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/indigo-to-launch-mumbai-istanbul-flights-from-jan-1-bookings-begin-122101101311_1.html</t>
+          <t>https://www.business-standard.com/budget/article/budget-to-be-carefully-structured-to-manage-growth-inflation-fm-122101201098_1.html</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>CAIiEJBKaQXsvR2XSJtsxiPAuI0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEI5KMo5JDkDCA7UahpJlNp8qGQgEKhAIACoHCAowsLXdCjCm3dEBMNPjpAM</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:58:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:53:00 GMT</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>IndiGo to launch Mumbai-Istanbul flights from Jan 1, bookings begins  Business Standard</t>
+          <t>Budget focus is to maintain growth, tame inflation: FM Nirmala Sitharaman  Business Standard</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -1953,27 +1953,27 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Who is D Y Chandrachud? - Business Standard</t>
+          <t>MEAs Dr Adarsh Swaika appointed Indias next ambassador to Kuwait - Business Standard</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/about/who-is-d-y-chandrachud</t>
+          <t>https://www.business-standard.com/article/current-affairs/mea-s-dr-adarsh-swaika-appointed-india-s-next-ambassador-to-kuwait-122101300019_1.html</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>CBMiPmh0dHBzOi8vd3d3LmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hYm91dC93aG8taXMtZC15LWNoYW5kcmFjaHVk0gEA</t>
+          <t>CAIiEMI1J_6x77_N7bFRsjABgkcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:09:19 GMT</t>
+          <t>Thu, 13 Oct 2022 01:22:00 GMT</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Who is D Y Chandrachud?  Business Standard</t>
+          <t>MEAs Dr Adarsh Swaika appointed Indias next ambassador to Kuwait  Business Standard</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -1989,27 +1989,27 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Effective directors display the art of healthy scepticism - Business Standard</t>
+          <t>Fireside Ventures announces $225-mn fund for investment in Indian startups - Business Standard</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/opinion/effective-directors-display-the-art-of-healthy-scepticism-122101101345_1.html</t>
+          <t>https://www.business-standard.com/article/companies/fireside-ventures-announces-225-mn-fund-for-investment-in-indian-startups-122101201251_1.html</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>CAIiEDMjSYtksbU0peDwUIDAXhwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEC3O6oGLBL4wK5DbANw37wcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:09:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:31:00 GMT</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Effective directors display the art of healthy scepticism  Business Standard</t>
+          <t>Fireside Ventures announces $225-mn fund for investment in Indian startups  Business Standard</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2025,27 +2025,27 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>TCS launches solution to help central banks in use of digital currenciess - Business Standard</t>
+          <t>LIC sells over 2% stake in Power Grid for Rs 3,079 crore in 5 months - Business Standard</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/tcs-launches-solution-to-help-central-banks-in-use-of-digital-currencies-122101101292_1.html</t>
+          <t>https://www.business-standard.com/article/companies/lic-sells-over-2-stake-in-power-grid-for-rs-3-079-crore-in-5-months-122101201231_1.html</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>CAIiEM0QPpedn1GQOyFaOiALnzsqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiENDjQ_YHeN6sZcNUhQcHfSwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:26:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:47:00 GMT</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>TCS launches solution to help central banks in use of digital currenciess  Business Standard</t>
+          <t>LIC sells over 2% stake in Power Grid for Rs 3,079 crore in 5 months  Business Standard</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2061,27 +2061,27 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>High life in the death zone of the forgotten guardians of Everests - Business Standard</t>
+          <t>High food prices push retail inflation to 5-month high of 7.41% in Sept - Business Standard</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/beyond-business/high-life-in-the-death-zone-of-the-forgotten-guardians-of-everest-122101101343_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/retail-inflation-accelerates-to-7-41-in-sept-iip-contracts-0-8-in-aug-122101200923_1.html</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>CAIiEHhXsgxZQvuYjUgGGLOreRcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CBMikgFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9lY29ub215LXBvbGljeS9yZXRhaWwtaW5mbGF0aW9uLWFjY2VsZXJhdGVzLXRvLTctNDEtaW4tc2VwdC1paXAtY29udHJhY3RzLTAtOC1pbi1hdWctMTIyMTAxMjAwOTIzXzEuaHRtbNIBAA</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 17:02:00 GMT</t>
+          <t>Wed, 12 Oct 2022 12:25:00 GMT</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>High life in the death zone of the forgotten guardians of Everests  Business Standard</t>
+          <t>High food prices push retail inflation to 5-month high of 7.41% in Sept  Business Standard</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2097,27 +2097,27 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>DoT summons mobile device makers, telecom companies to push 5G updatess - Business Standard</t>
+          <t>Dabolim airport to shut if app-based transport not supported: Goa Minister - Business Standard</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/dot-summons-mobile-device-makers-telecom-companies-to-push-5g-updates-122101101133_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/dabolim-airport-to-shut-if-app-based-transport-not-supported-goa-minister-122101201210_1.html</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>CAIiEM_jKMbOhos5DNvCuqZK-r0qGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiEDdoLIHEvigxVHcRq2-0IRMqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:19:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:21:00 GMT</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>DoT summons mobile device makers, telecom companies to push 5G updatess  Business Standard</t>
+          <t>Dabolim airport to shut if app-based transport not supported: Goa Minister  Business Standard</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2133,27 +2133,27 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sebi gives go-ahead to HSBC AMCs acquisition of L&amp;T Investment Managerss - Business Standard</t>
+          <t>Despite recessionary trends… were talking about 7% growth: Hiranandani - Business Standard</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/markets/sebi-gives-go-ahead-to-hsbc-amc-s-acquisition-of-l-t-investment-managers-122101101176_1.html</t>
+          <t>https://www.business-standard.com/article/companies/real-estate-sector-will-sustain-growth-momentum-niranjan-hiranandani-122101200910_1.html</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>CAIiEMdr0PNtBAohyHcljalzrDcqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CBMijAFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jb21wYW5pZXMvcmVhbC1lc3RhdGUtc2VjdG9yLXdpbGwtc3VzdGFpbi1ncm93dGgtbW9tZW50dW0tbmlyYW5qYW4taGlyYW5hbmRhbmktMTIyMTAxMjAwOTEwXzEuaHRtbNIBkAFodHRwczovL3dhcC5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS1hbXAvY29tcGFuaWVzL3JlYWwtZXN0YXRlLXNlY3Rvci13aWxsLXN1c3RhaW4tZ3Jvd3RoLW1vbWVudHVtLW5pcmFuamFuLWhpcmFuYW5kYW5pLTEyMjEwMTIwMDkxMF8xLmh0bWw</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:53:00 GMT</t>
+          <t>Wed, 12 Oct 2022 12:22:00 GMT</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Sebi gives go-ahead to HSBC AMCs acquisition of L&amp;T Investment Managerss  Business Standard</t>
+          <t>Despite recessionary trends… were talking about 7% growth: Hiranandani  Business Standard</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2169,27 +2169,27 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Chinese carmaker BYD drives into Indian e-SUV segment with Atto 3s - Business Standard</t>
+          <t>Still looking for free trade deal with India by Diwali, says Britain - Business Standard</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/automobile/chinese-carmaker-byd-enters-e-suv-segment-with-electric-atto-3-122101101152_1.html</t>
+          <t>https://www.business-standard.com/article/politics/still-looking-for-free-trade-deal-with-india-by-diwali-says-britain-122101201297_1.html</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>CAIiEOezu6ZB1jZto8XnxQBXItMqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEM0Yk1QNTukRP7vu73gxLhMqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:00:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:29:00 GMT</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Chinese carmaker BYD drives into Indian e-SUV segment with Atto 3s  Business Standard</t>
+          <t>Still looking for free trade deal with India by Diwali, says Britain  Business Standard</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2205,27 +2205,27 @@
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Results preview: Order-book booster to stay for capital goods firmss - Business Standard</t>
+          <t>Bihar Board releases DElEd result for first and second year exams - Business Standard</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/q2-preview-order-book-booster-to-continue-for-capital-goods-firms-122101100980_1.html</t>
+          <t>https://www.business-standard.com/article/education/bihar-board-releases-deled-result-for-first-and-second-year-exams-122101201348_1.html</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>CAIiEDry1idSeEOYt8C7Hm5BzWgqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEFPmjqTwTwGf-jSoqpFKEi8qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:24:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:15:00 GMT</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Results preview: Order-book booster to stay for capital goods firmss  Business Standard</t>
+          <t>Bihar Board releases DElEd result for first and second year exams  Business Standard</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2241,27 +2241,27 @@
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Liquidity slips into deficit on high credit growth, festival loan demands - Business Standard</t>
+          <t>Hong Kong Market falls 0.8% - Business Standard</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/finance/liquidity-slips-into-deficit-on-high-credit-growth-festival-loan-demand-122101101169_1.html</t>
+          <t>https://www.business-standard.com/article/news-cm/hong-kong-market-falls-0-8-122101201336_1.html</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>CAIiEButnuchCV6J0_Lt1F7K-lwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CBMiYGh0dHBzOi8vd3d3LmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlL25ld3MtY20vaG9uZy1rb25nLW1hcmtldC1mYWxscy0wLTgtMTIyMTAxMjAxMzM2XzEuaHRtbNIBZGh0dHBzOi8vd2FwLmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlLWFtcC9uZXdzLWNtL2hvbmcta29uZy1tYXJrZXQtZmFsbHMtMC04LTEyMjEwMTIwMTMzNl8xLmh0bWw</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:04:00 GMT</t>
+          <t>Wed, 12 Oct 2022 11:49:00 GMT</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Liquidity slips into deficit on high credit growth, festival loan demands  Business Standard</t>
+          <t>Hong Kong Market falls 0.8%  Business Standard</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2277,27 +2277,27 @@
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>GSTs secret sauce: Tax collections continue to surge but for how long?s - Business Standard</t>
+          <t>Govt forms panel to study WHO reports on deaths linked to 4 Indian syrups - Business Standard</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/opinion/gst-s-secret-sauce-tax-collections-continue-to-surge-but-for-how-long-122101101338_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/govt-forms-panel-to-study-who-reports-on-deaths-linked-to-4-indian-syrups-122101201094_1.html</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>CAIiEIUKBdfnTLKFyu0oXljDHa0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiECYvj-YfBrUA6rPaegXosxYqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:44:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:06:00 GMT</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>GSTs secret sauce: Tax collections continue to surge but for how long?s  Business Standard</t>
+          <t>Govt forms panel to study WHO reports on deaths linked to 4 Indian syrups  Business Standard</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2313,27 +2313,27 @@
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ineffective implementation: Ban on single-use plastic is not workings - Business Standard</t>
+          <t>Govt okays Rs 22,000 crore one-time grant for OMCs to battle losses - Business Standard</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/opinion/ineffective-implementation-ban-on-single-use-plastic-is-not-working-122101101335_1.html</t>
+          <t>https://www.business-standard.com/article/companies/cabinet-approves-rs-22-000-crore-one-time-grant-for-omcs-to-battle-losses-122101201078_1.html</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>CAIiEKbX2DCP6GQzeXaSe26CRWoqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CBMikQFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jb21wYW5pZXMvY2FiaW5ldC1hcHByb3Zlcy1ycy0yMi0wMDAtY3JvcmUtb25lLXRpbWUtZ3JhbnQtZm9yLW9tY3MtdG8tYmF0dGxlLWxvc3Nlcy0xMjIxMDEyMDEwNzhfMS5odG1s0gEA</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:38:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:47:00 GMT</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Ineffective implementation: Ban on single-use plastic is not workings  Business Standard</t>
+          <t>Govt okays Rs 22,000 crore one-time grant for OMCs to battle losses  Business Standard</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2349,27 +2349,27 @@
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Fire-fighting Bank of England forced to buy inflation-linked bondss - Business Standard</t>
+          <t>State Bank of India, HDFC cut home loan rates to 8.4% for new applicants - Business Standard</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/fire-fighting-bank-of-england-forced-to-buy-inflation-linked-bonds-122101100800_1.html</t>
+          <t>https://www.business-standard.com/article/finance/sbi-slashes-home-loan-rate-up-to-25-basis-points-in-festive-season-122101201109_1.html</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>CBMijgFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9pbnRlcm5hdGlvbmFsL2ZpcmUtZmlnaHRpbmctYmFuay1vZi1lbmdsYW5kLWZvcmNlZC10by1idXktaW5mbGF0aW9uLWxpbmtlZC1ib25kcy0xMjIxMDExMDA4MDBfMS5odG1s0gEA</t>
+          <t>CAIiEDXBM2ZbAWYAkELztJu1o8UqGQgEKhAIACoHCAowsLXdCjCm3dEBMMPjpAM</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 10:52:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:56:00 GMT</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Fire-fighting Bank of England forced to buy inflation-linked bondss  Business Standard</t>
+          <t>State Bank of India, HDFC cut home loan rates to 8.4% for new applicants  Business Standard</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2385,27 +2385,27 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Experts debate fugitive diamantaire Nirav Modis suicide risk in UK courts - Business Standard</t>
+          <t>RBI to submit report on failure to tackle inflation for 3 qtrs since Jan - Business Standard</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/experts-debate-fugitive-diamantaire-nirav-modi-s-suicide-risk-in-uk-court-122101101337_1.html</t>
+          <t>https://www.business-standard.com/article/finance/rbi-to-submit-report-on-failure-to-tackle-inflation-for-3-qtrs-since-jan-122101201083_1.html</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>CAIiED1NmJf-tisFdvU30OTudUMqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEJmdRDH4lNAt1P9kx46DNqoqGQgEKhAIACoHCAowsLXdCjCm3dEBMMPjpAM</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:42:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:07:00 GMT</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Experts debate fugitive diamantaire Nirav Modis suicide risk in UK courts  Business Standard</t>
+          <t>RBI to submit report on failure to tackle inflation for 3 qtrs since Jan  Business Standard</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2421,27 +2421,27 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Binny files nomination for post of BCCI prez, Shah likely to remain secys - Business Standard</t>
+          <t>China Market rebounds on strong loan data - Business Standard</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/binny-files-nomination-for-post-of-bcci-prez-shah-likely-to-remain-secy-122101101032_1.html</t>
+          <t>https://www.business-standard.com/article/news-cm/china-market-rebounds-on-strong-loan-data-122101201317_1.html</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>CAIiEPDUHDGvjS-1E5xLpbl6lpgqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CBMib2h0dHBzOi8vd3d3LmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlL25ld3MtY20vY2hpbmEtbWFya2V0LXJlYm91bmRzLW9uLXN0cm9uZy1sb2FuLWRhdGEtMTIyMTAxMjAxMzE3XzEuaHRtbNIBc2h0dHBzOi8vd2FwLmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlLWFtcC9uZXdzLWNtL2NoaW5hLW1hcmtldC1yZWJvdW5kcy1vbi1zdHJvbmctbG9hbi1kYXRhLTEyMjEwMTIwMTMxN18xLmh0bWw</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:25:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:46:03 GMT</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Binny files nomination for post of BCCI prez, Shah likely to remain secys  Business Standard</t>
+          <t>China Market rebounds on strong loan data  Business Standard</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2457,27 +2457,27 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Industry body Nasscom launches responsible AI hub and resource kits - Business Standard</t>
+          <t>Shareholders of PVR approve the proposed merger with Inox Leisure - Business Standard</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/industry-body-nasscom-launches-responsible-ai-hub-and-resource-kit-122101101312_1.html</t>
+          <t>https://www.business-standard.com/article/companies/multiplex-operator-pvr-shareholders-approve-merger-with-inox-leisure-122101201031_1.html</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>CAIiEGMsF97OoVI2hZ4efq9XgNwqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEF14tloIkBvnSBLj2rDMUckqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:30:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:24:00 GMT</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Industry body Nasscom launches responsible AI hub and resource kits  Business Standard</t>
+          <t>Shareholders of PVR approve the proposed merger with Inox Leisure  Business Standard</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2493,27 +2493,27 @@
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Goa to face loss of Rs 500 cr if visa restriction to UK not relaxed: GFPs - Business Standard</t>
+          <t>Uber, Ola, Rapido continue auto services despite Karnataka govts ban - Business Standard</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/goa-to-face-loss-of-rs-500-cr-if-visa-restriction-to-uk-not-relaxed-gfp-122101101302_1.html</t>
+          <t>https://www.business-standard.com/article/companies/uber-ola-continue-auto-rickshaw-services-despite-karnataka-govt-s-ban-122101201262_1.html</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>CAIiEHghaE75tWo0kKdx04pa7wEqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiENxGyjjB7FlhP-PNBGiUodcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:27:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:22:00 GMT</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Goa to face loss of Rs 500 cr if visa restriction to UK not relaxed: GFPs  Business Standard</t>
+          <t>Uber, Ola, Rapido continue auto services despite Karnataka govts ban  Business Standard</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2529,27 +2529,27 @@
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Indian jute making its way - from US markets to Italy wine producerss - Business Standard</t>
+          <t>Centre approves development of a container terminal in Kandla Port - Business Standard</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/indian-jute-making-its-way-from-us-markets-to-italy-wine-producers-122101101329_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/cabinet-approves-rs-4-244-crore-container-terminal-in-kandla-port-122101201039_1.html</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>CAIiENd4qpgYOxfzt2y9pkqc6WwqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEIAtfqbaUqDCjzeMaH9ZmfMqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:25:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:50:00 GMT</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Indian jute making its way - from US markets to Italy wine producerss  Business Standard</t>
+          <t>Centre approves development of a container terminal in Kandla Port  Business Standard</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2565,27 +2565,27 @@
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Life insurers new biz premium up 17% at Rs 36367 cr in September: Irdais - Business Standard</t>
+          <t>Reflections on life and success, without flashy mantras - Business Standard</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/finance/life-insurers-new-biz-premium-up-17-at-rs-36-367-cr-in-september-irdai-122101101307_1.html</t>
+          <t>https://www.business-standard.com/article/beyond-business/reflections-on-life-and-success-without-flashy-mantras-122101201346_1.html</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>CAIiEFnlyDd4Bysb3QTtOoNh5L4qGQgEKhAIACoHCAowsLXdCjCm3dEBMMPjpAM</t>
+          <t>CAIiEIyX32jt7K59unmrDxfInHAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:21:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:06:00 GMT</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Life insurers new biz premium up 17% at Rs 36367 cr in September: Irdais  Business Standard</t>
+          <t>Reflections on life and success, without flashy mantras  Business Standard</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2601,27 +2601,27 @@
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MDs, CEOs of ARCs cant have more than 3 terms in office without a cool-offs - Business Standard</t>
+          <t>One year of PM-GatiShakti: National masterplan drives infra projects - Business Standard</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/finance/rbi-mandates-office-tenure-and-retirement-age-limit-for-arc-ceos-122101101247_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/1-year-of-pm-gatishakti-national-masterplan-gives-boost-to-infra-projects-122101201110_1.html</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>CAIiEElvJ4iFJaqclh-y1UU7UAAqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiEDSyCsrCpVjmdElFoj3Zso0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:07:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:17:00 GMT</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>MDs, CEOs of ARCs cant have more than 3 terms in office without a cool-offs  Business Standard</t>
+          <t>One year of PM-GatiShakti: National masterplan drives infra projects  Business Standard</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2637,27 +2637,27 @@
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Ukraine-Russia conflict: Experts assess Crimean bridge blast damages - Business Standard</t>
+          <t>Govt may clear semiconductor unit proposals in next 30-60 days: MoS IT - Business Standard</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/ukraine-russia-conflict-experts-assess-crimean-bridge-blast-damage-122101100322_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/govt-may-clear-semiconductor-unit-proposals-in-next-30-60-days-mos-it-122101201113_1.html</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>CAIiEHc0Vwp8JpMZFNNNm2GhvXEqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEKP7dPUtA9agVJ1LRO2WlM0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 05:25:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:01:00 GMT</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Ukraine-Russia conflict: Experts assess Crimean bridge blast damages  Business Standard</t>
+          <t>Govt may clear semiconductor unit proposals in next 30-60 days: MoS IT  Business Standard</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -2673,27 +2673,27 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>UIDAI urges document updation for Aadhaar numbers issued over 10 yrs backs - Business Standard</t>
+          <t>NHAI INvIT raises Rs 1,430 crore for funding acquisition of road projects - Business Standard</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/uidai-urges-document-updation-for-aadhaar-numbers-issued-over-10-yrs-back-122101101281_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/nhai-invit-raises-rs-1-430-crore-for-funding-acquisition-of-road-projects-122101201192_1.html</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>CAIiEIaJ6tHk49AgQ41yc0biRccqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEC3e5oKbEdQNJ880ceo61bcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:04:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:51:00 GMT</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>UIDAI urges document updation for Aadhaar numbers issued over 10 yrs backs  Business Standard</t>
+          <t>NHAI INvIT raises Rs 1,430 crore for funding acquisition of road projects  Business Standard</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -2709,27 +2709,27 @@
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Google takes on lease 464000 sq ft space at Adani data centre in Noidas - Business Standard</t>
+          <t>Govt permits exporters to ship raw sugar to US under TRQ till Dec 31 - Business Standard</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/google-takes-on-lease-464-000-sq-ft-space-at-adani-data-centre-in-noida-122101101273_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/govt-permits-exporters-to-ship-raw-sugar-to-us-under-trq-till-dec-31-122101200599_1.html</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>CAIiEOJ4VsfIGVMdKapMiBuZtq8qGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEHfxYaojtTWmCtFOz3AGVbEqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:02:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:05:00 GMT</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Google takes on lease 464000 sq ft space at Adani data centre in Noidas  Business Standard</t>
+          <t>Govt permits exporters to ship raw sugar to US under TRQ till Dec 31  Business Standard</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -2745,27 +2745,27 @@
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>AirAsia India planes fairing panel found missing; DGCA orders probes - Business Standard</t>
+          <t>CCPA issues notices for surrogate ads to Kamla Pasand, Rajnigandha - Business Standard</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/airasia-india-plane-s-fairing-panel-found-missing-dgca-orders-probe-122101101282_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/ccpa-issues-notices-for-surrogate-advertising-to-brands-of-various-products-122101201197_1.html</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>CAIiEBKs3MHFNT0GRfkFCMkjje4qGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEKLjoHBtQEvtGfnW37WBU9gqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:05:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:04:00 GMT</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>AirAsia India planes fairing panel found missing; DGCA orders probes  Business Standard</t>
+          <t>CCPA issues notices for surrogate ads to Kamla Pasand, Rajnigandha  Business Standard</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -2781,27 +2781,27 @@
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Samsung announces discounts on Galaxy Z Flip 3, Galaxy Z Fold 3 foldabless - Business Standard</t>
+          <t>FDI and the ordinary Indian - Business Standard</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://wap.business-standard.com/article/technology/samsung-announces-discounts-on-galaxy-z-flip-3-galaxy-z-fold-3-foldables-122101100949_1.html</t>
+          <t>https://www.business-standard.com/article/opinion/fdi-and-the-ordinary-indian-122101201338_1.html</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>CAIiEH1jkGCUa71HHId6hasqYpMqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiEAQ_lHM62ASVScBnQK3yVkAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 12:38:00 GMT</t>
+          <t>Wed, 12 Oct 2022 17:03:00 GMT</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Samsung announces discounts on Galaxy Z Flip 3, Galaxy Z Fold 3 foldabless  Business Standard</t>
+          <t>FDI and the ordinary Indian  Business Standard</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -2817,27 +2817,27 @@
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>United Nations will become 'irrelevant' without reforms: Jaishankar - Business Standard</t>
+          <t>Xi all set to rewind Chinas clock back to one leader rule of Mao era - Business Standard</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/united-nations-will-become-irrelevant-without-reforms-jaishankar-122101101242_1.html</t>
+          <t>https://www.business-standard.com/article/international/xi-all-set-to-rewind-china-s-clock-back-to-one-leader-rule-of-mao-era-122101200806_1.html</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>CBMijgFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jdXJyZW50LWFmZmFpcnMvdW5pdGVkLW5hdGlvbnMtd2lsbC1iZWNvbWUtaXJyZWxldmFudC13aXRob3V0LXJlZm9ybXMtamFpc2hhbmthci0xMjIxMDExMDEyNDJfMS5odG1s0gEA</t>
+          <t>CAIiEAyQhwkB2IwyZrRJGHNztzwqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:02:00 GMT</t>
+          <t>Wed, 12 Oct 2022 12:53:00 GMT</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>United Nations will become 'irrelevant' without reforms: Jaishankar  Business Standard</t>
+          <t>Xi all set to rewind Chinas clock back to one leader rule of Mao era  Business Standard</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -2853,27 +2853,27 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Sale of cement units to Adani group a relief for Jaiprakash lenderss - Business Standard</t>
+          <t>European stocks struggle for direction, sterling recovers after BoE warning - Business Standard</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/cement-unit-sale-to-help-jaiprakash-associates-lenders-to-get-dues-122101101204_1.html</t>
+          <t>https://www.business-standard.com/article/international/european-stocks-struggle-for-direction-sterling-recovers-after-boe-warning-122101200626_1.html</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>CAIiEEz72OtHZPXuzRFtja-GZ-IqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEFIi72TtmQ1cNmu60JAXHZEqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:42:00 GMT</t>
+          <t>Wed, 12 Oct 2022 10:02:00 GMT</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Sale of cement units to Adani group a relief for Jaiprakash lenderss  Business Standard</t>
+          <t>European stocks struggle for direction, sterling recovers after BoE warning  Business Standard</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -2889,27 +2889,27 @@
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Fast-track mechanism on the cards to help Indian investors in UAEs - Business Standard</t>
+          <t>Southern Railway division introduces QR-based booking system at 61 stations - Business Standard</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/fast-track-mechanism-on-the-cards-to-help-indian-investors-in-uae-122101101095_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/southern-railway-division-introduces-qr-based-booking-system-at-61-stations-122101201173_1.html</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>CAIiEF2ShwJ-n5V5FOEanYnb404qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEC85YLHDOjno7U9_g0-fTroqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:13:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:56:00 GMT</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Fast-track mechanism on the cards to help Indian investors in UAEs  Business Standard</t>
+          <t>Southern Railway division introduces QR-based booking system at 61 stations  Business Standard</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -2925,27 +2925,27 @@
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Bollywood stars, corporate bosses fire up Mumbai, Delhi luxury house mktss - Business Standard</t>
+          <t>BS Number Wise: A strategy for non-strategic state firms as losses mount - Business Standard</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/luxury-property-deals-by-bollywood-celebrities-cxos-up-since-2021-122101000751_1.html</t>
+          <t>https://www.business-standard.com/article/companies/bs-number-wise-a-strategy-for-non-strategic-state-firms-as-losses-mount-122101201328_1.html</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>CAIiEFf5SzIi7u0_dP-PuPWRSR4qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEKIBZ5vtcNVKuts7ZYSixQAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:50:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:53:00 GMT</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Bollywood stars, corporate bosses fire up Mumbai, Delhi luxury house mktss  Business Standard</t>
+          <t>BS Number Wise: A strategy for non-strategic state firms as losses mount  Business Standard</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -2961,27 +2961,27 @@
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Mumbai logs 129 new Covid-19 cases, no death; active tally at 881s - Business Standard</t>
+          <t>Oil &amp; Gas: A discouraging history - Business Standard</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/mumbai-logs-129-new-covid-19-cases-no-death-active-tally-at-881-122101101264_1.html</t>
+          <t>https://www.business-standard.com/article/opinion/oil-gas-a-discouraging-history-122101201331_1.html</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>CAIiECivKGgTtJiXvEZ3u1NIm5EqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEMSLMocjKLofOdqZtTaH9g0qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 16:01:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:55:00 GMT</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Mumbai logs 129 new Covid-19 cases, no death; active tally at 881s  Business Standard</t>
+          <t>Oil &amp; Gas: A discouraging history  Business Standard</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -2997,27 +2997,27 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>There is no single silver bullet behind crash detection, says Apples - Business Standard</t>
+          <t>Heres why Adani Wilmar expects Q2 revenue growth in low single digit - Business Standard</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/technology/there-is-no-single-silver-bullet-behind-crash-detection-says-apple-122101100372_1.html</t>
+          <t>https://www.business-standard.com/article/companies/here-s-why-adani-wilmar-expects-q2-revenue-growth-in-low-single-digit-122101201322_1.html</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>CAIiEOiRjDv3mElDFw-0OzGLPUEqGQgEKhAIACoHCAowsLXdCjCm3dEBMPTgpAM</t>
+          <t>CAIiEKwRLtq38x8JPFrNX1lLTK0qGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 09:31:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:57:00 GMT</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>There is no single silver bullet behind crash detection, says Apples  Business Standard</t>
+          <t>Heres why Adani Wilmar expects Q2 revenue growth in low single digit  Business Standard</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3033,27 +3033,27 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Flight bookings to Qatar boom for FIFA World Cup, especially from Dubais - Business Standard</t>
+          <t>Black swan events in global markets upset Indias long-term LNG story - Business Standard</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://wap.business-standard.com/article/international/flight-bookings-to-qatar-boom-for-fifa-world-cup-especially-from-dubai-122101100795_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/black-swans-in-global-markets-puncture-india-s-long-term-lng-story-122101200944_1.html</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>CAIiEA1Sm7tav_Qgi4lpuI55TuUqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEAAkphaD9UpraluDh66gGo8qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 10:50:00 GMT</t>
+          <t>Wed, 12 Oct 2022 12:37:00 GMT</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Flight bookings to Qatar boom for FIFA World Cup, especially from Dubais  Business Standard</t>
+          <t>Black swan events in global markets upset Indias long-term LNG story  Business Standard</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3069,27 +3069,27 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Japanese automaker Nissan says it is pulling out of Russia amid wars - Business Standard</t>
+          <t>Samsung likely to offer 5,000 mAh battery in upcoming Galaxy S23 Ultra - Business Standard</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/japanese-automaker-nissan-says-it-is-pulling-out-of-russia-amid-war-122101100918_1.html</t>
+          <t>https://www.business-standard.com/article/technology/samsung-likely-to-offer-5-000-mah-battery-in-upcoming-galaxy-s23-ultra-122101200815_1.html</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>CAIiEHCm7WDTw7lX03rGwuTOgHYqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEKjjbKwkYJEdvXicVUlqBBcqGQgEKhAIACoHCAowsLXdCjCm3dEBMPTgpAM</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 12:49:00 GMT</t>
+          <t>Wed, 12 Oct 2022 13:56:00 GMT</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Japanese automaker Nissan says it is pulling out of Russia amid wars  Business Standard</t>
+          <t>Samsung likely to offer 5,000 mAh battery in upcoming Galaxy S23 Ultra  Business Standard</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3105,27 +3105,27 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Market slides for 3rd day, Sensex drops 844 pts, Nifty ends below 17000 marks - Business Standard</t>
+          <t>Maharashtra records 476 new Covid-19 cases, 4 deaths; active tally at 2,455 - Business Standard</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/news-cm/market-slides-for-3rd-day-sensex-drops-844-pts-nifty-ends-below-17-000-mark-122101100864_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/maharashtra-records-476-new-covid-19-cases-4-deaths-active-tally-at-2-455-122101201219_1.html</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>CBMikQFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9uZXdzLWNtL21hcmtldC1zbGlkZXMtZm9yLTNyZC1kYXktc2Vuc2V4LWRyb3BzLTg0NC1wdHMtbmlmdHktZW5kcy1iZWxvdy0xNy0wMDAtbWFyay0xMjIxMDExMDA4NjRfMS5odG1s0gEA</t>
+          <t>CAIiEDstv9zgYz0nEpKTuRVOTbUqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 11:27:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:38:00 GMT</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Market slides for 3rd day, Sensex drops 844 pts, Nifty ends below 17000 marks  Business Standard</t>
+          <t>Maharashtra records 476 new Covid-19 cases, 4 deaths; active tally at 2,455  Business Standard</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3141,27 +3141,27 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Indian-origin Sikh on trial for $10.4-mn crypto bungle in Melbournes - Business Standard</t>
+          <t>Australia Stocks end mixed - Business Standard</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/markets/indian-origin-sikh-on-trial-for-10-4-mn-crypto-bungle-in-melbourne-122101101187_1.html</t>
+          <t>https://www.business-standard.com/article/news-cm/australia-stocks-end-mixed-122101201303_1.html</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>CAIiEC_g_2ibif2BmyozBimfHQ4qGQgEKhAIACoHCAowsLXdCjCm3dEBMLPjpAM</t>
+          <t>CBMiYGh0dHBzOi8vd3d3LmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlL25ld3MtY20vYXVzdHJhbGlhLXN0b2Nrcy1lbmQtbWl4ZWQtMTIyMTAxMjAxMzAzXzEuaHRtbNIBZGh0dHBzOi8vd2FwLmJ1c2luZXNzLXN0YW5kYXJkLmNvbS9hcnRpY2xlLWFtcC9uZXdzLWNtL2F1c3RyYWxpYS1zdG9ja3MtZW5kLW1peGVkLTEyMjEwMTIwMTMwM18xLmh0bWw</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:00:00 GMT</t>
+          <t>Wed, 12 Oct 2022 11:24:00 GMT</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Indian-origin Sikh on trial for $10.4-mn crypto bungle in Melbournes  Business Standard</t>
+          <t>Australia Stocks end mixed  Business Standard</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3177,27 +3177,27 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Indias first Covid cure Vincov-19 completes second phase clinical trials - Business Standard</t>
+          <t>India-UK trade deal on verge of collapse over visa comments: Report - Business Standard</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/vincov-19-country-s-first-anti-dote-for-covid-completes-phase-2-trials-122101101163_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/india-uk-trade-deal-on-verge-of-collapse-over-visa-comments-report-122101201205_1.html</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>CAIiEAuDsRyPfFbhqhn-dQ2f4ukqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiECGePQoPOdKLyfABFS0wELEqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:15:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:30:00 GMT</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Indias first Covid cure Vincov-19 completes second phase clinical trials  Business Standard</t>
+          <t>India-UK trade deal on verge of collapse over visa comments: Report  Business Standard</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3213,27 +3213,27 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Dhoni picks up equity in plant-based protein startup Shaka Harrys - Business Standard</t>
+          <t>West Bengal govt hands over Letter of Award for Tajpur port to Adani Ports - Business Standard</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/dhoni-picks-up-equity-in-plant-based-protein-startup-shaka-harry-122101101182_1.html</t>
+          <t>https://www.business-standard.com/article/companies/bengal-government-hands-over-letter-of-award-for-tajpur-port-to-adani-ports-122101201271_1.html</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>CAIiECOD5Xp087-AzFIrByyEvQgqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEK3sWdkC5nxcy84u8QSDHXcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:01:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:11:00 GMT</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Dhoni picks up equity in plant-based protein startup Shaka Harrys  Business Standard</t>
+          <t>West Bengal govt hands over Letter of Award for Tajpur port to Adani Ports  Business Standard</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3249,27 +3249,27 @@
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SC appointments: What is the collegium system, and how does it work?s - Business Standard</t>
+          <t>HCLTech restructures the top management with a new COO and CHRO - Business Standard</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/sc-appointments-what-is-the-collegium-system-and-how-does-it-work-122101100824_1.html</t>
+          <t>https://www.business-standard.com/article/companies/hcltech-restructures-the-top-management-with-a-new-coo-and-chro-122101201278_1.html</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>CAIiECsvgk3Sqspmg7jePweAhBAqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
+          <t>CAIiEHTALARd287R2qeBrHz0mScqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 11:15:00 GMT</t>
+          <t>Wed, 12 Oct 2022 16:25:00 GMT</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>SC appointments: What is the collegium system, and how does it work?s  Business Standard</t>
+          <t>HCLTech restructures the top management with a new COO and CHRO  Business Standard</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -3285,27 +3285,27 @@
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Route One Fund sells 1.54% stake in IndusInd Bank for Rs 1401 crs - Business Standard</t>
+          <t>Intel plans major layoffs this month as PC sales nosedive globally: Report - Business Standard</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/markets/route-one-fund-sells-1-54-stake-in-indusind-bank-for-rs-1-401-cr-122101101195_1.html</t>
+          <t>https://www.business-standard.com/article/international/intel-plans-major-layoffs-this-month-as-pc-sales-nosedive-globally-report-122101200731_1.html</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>CAIiEAa24AMUoWUywj__EpRjmXgqGQgEKhAIACoHCAowsLXdCjCm3dEBMLPjpAM</t>
+          <t>CAIiEEt2HJ7BBlmAi3lds-awOkYqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:04:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:03:00 GMT</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Route One Fund sells 1.54% stake in IndusInd Bank for Rs 1401 crs  Business Standard</t>
+          <t>Intel plans major layoffs this month as PC sales nosedive globally: Report  Business Standard</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -3321,27 +3321,27 @@
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
-          <t>India emerges as positive spot due to policy responses, says ex-CEAs - Business Standard</t>
+          <t>HCLTech revenue growth guidance raised to 13.5-14.5%; Q2 profit up 7% - Business Standard</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/india-emerges-as-positive-spot-due-to-policy-responses-says-ex-cea-122101101192_1.html</t>
+          <t>https://www.business-standard.com/article/companies/hcl-tech-q2-net-profit-jumps-7-to-rs-3-258-crore-revenue-grows-19-5-122101200953_1.html</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>CAIiEMazOjLgYETT-rxVuglh1zIqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEPYMZhMh_4Fua9TjJaapWpoqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 15:06:00 GMT</t>
+          <t>Wed, 12 Oct 2022 13:22:00 GMT</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>India emerges as positive spot due to policy responses, says ex-CEAs  Business Standard</t>
+          <t>HCLTech revenue growth guidance raised to 13.5-14.5%; Q2 profit up 7%  Business Standard</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -3357,27 +3357,27 @@
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Suzlon secures 144.9 MW wind power order from Aditya Birla Groups - Business Standard</t>
+          <t>Russia ready to resume gas supplies to EU via Nord Stream 2: Putin - Business Standard</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/suzlon-secures-144-9-mw-wind-power-order-from-aditya-birla-group-122101101178_1.html</t>
+          <t>https://www.business-standard.com/article/international/vladimir-putin-says-russia-could-increase-gas-supplies-to-europe-122101200814_1.html</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>CAIiEMWeKAdR8_2v9ow4lF2Cz5gqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CBMijAFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9pbnRlcm5hdGlvbmFsL3ZsYWRpbWlyLXB1dGluLXNheXMtcnVzc2lhLWNvdWxkLWluY3JlYXNlLWdhcy1zdXBwbGllcy10by1ldXJvcGUtMTIyMTAxMjAwODE0XzEuaHRtbNIBkAFodHRwczovL3dhcC5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS1hbXAvaW50ZXJuYXRpb25hbC92bGFkaW1pci1wdXRpbi1zYXlzLXJ1c3NpYS1jb3VsZC1pbmNyZWFzZS1nYXMtc3VwcGxpZXMtdG8tZXVyb3BlLTEyMjEwMTIwMDgxNF8xLmh0bWw</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:56:00 GMT</t>
+          <t>Wed, 12 Oct 2022 11:44:00 GMT</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Suzlon secures 144.9 MW wind power order from Aditya Birla Groups  Business Standard</t>
+          <t>Russia ready to resume gas supplies to EU via Nord Stream 2: Putin  Business Standard</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3393,27 +3393,27 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Marksans Pharma to acquire Tevapharm's bulk formulations business - Business Standard</t>
+          <t>Delhi sees seasons first fog; air quality enter poor category by weekend - Business Standard</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>https://wap.business-standard.com/article/companies/marksans-pharma-to-acquire-tevapharm-s-bulk-formulations-business-122101101184_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/delhi-sees-season-s-first-fog-air-quality-enter-poor-category-by-weekend-122101201059_1.html</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>CAIiEFKWM9SDDMUAO-1JY_YHfhoqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEAKZ66Pf90Hubwj_seAbtecqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:58:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:37:00 GMT</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Marksans Pharma to acquire Tevapharm's bulk formulations business  Business Standard</t>
+          <t>Delhi sees seasons first fog; air quality enter poor category by weekend  Business Standard</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3429,27 +3429,27 @@
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Congress outsourced contract of abusing me, says PM Modi in Rajkot rallys - Business Standard</t>
+          <t>RBI appropriately tightening monetary policy to fight inflation: IMF - Business Standard</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/congress-outsourced-contract-of-abusing-me-says-pm-modi-in-rajkot-rally-122101100557_1.html</t>
+          <t>https://www.business-standard.com/article/news-cm/rbi-appropriately-tightening-monetary-policy-to-fight-inflation-imf-122101200675_1.html</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>CAIiEKkpS27oqVyxNekGhyJACJAqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CBMiiQFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9uZXdzLWNtL3JiaS1hcHByb3ByaWF0ZWx5LXRpZ2h0ZW5pbmctbW9uZXRhcnktcG9saWN5LXRvLWZpZ2h0LWluZmxhdGlvbi1pbWYtMTIyMTAxMjAwNjc1XzEuaHRtbNIBjQFodHRwczovL3dhcC5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS1hbXAvbmV3cy1jbS9yYmktYXBwcm9wcmlhdGVseS10aWdodGVuaW5nLW1vbmV0YXJ5LXBvbGljeS10by1maWdodC1pbmZsYXRpb24taW1mLTEyMjEwMTIwMDY3NV8xLmh0bWw</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 08:27:00 GMT</t>
+          <t>Wed, 12 Oct 2022 09:46:00 GMT</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Congress outsourced contract of abusing me, says PM Modi in Rajkot rallys  Business Standard</t>
+          <t>RBI appropriately tightening monetary policy to fight inflation: IMF  Business Standard</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3465,27 +3465,27 @@
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr">
         <is>
-          <t>AstraZeneca's nasal Covid vaccine not as effective as expected: Study - Business Standard</t>
+          <t>Byjus to lay off 2,500 staffers, targets profitability by March - Business Standard</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/astrazeneca-s-nasal-covid-vaccine-not-as-effective-as-expected-study-122101101025_1.html</t>
+          <t>https://www.business-standard.com/article/companies/on-a-path-to-profitability-targets-to-achieve-by-march-2023-byju-s-122101200959_1.html</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>CAIiEPjCUtmsmKkv2G0FBnkHo0kqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CBMiigFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jb21wYW5pZXMvb24tYS1wYXRoLXRvLXByb2ZpdGFiaWxpdHktdGFyZ2V0cy10by1hY2hpZXZlLWJ5LW1hcmNoLTIwMjMtYnlqdS1zLTEyMjEwMTIwMDk1OV8xLmh0bWzSAQA</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:44:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:45:00 GMT</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>AstraZeneca's nasal Covid vaccine not as effective as expected: Study  Business Standard</t>
+          <t>Byjus to lay off 2,500 staffers, targets profitability by March  Business Standard</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -3501,27 +3501,27 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Apartments sales in 7 cities at 161k units in Jan-Sep; highest since 2015s - Business Standard</t>
+          <t>Avoid sectors having global exposure like IT, oil, gas: ICICI Securities - Business Standard</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/apartments-sales-in-7-cities-at-161k-units-in-jan-sep-highest-since-2015-122101101089_1.html</t>
+          <t>https://www.business-standard.com/article/markets/avoid-sectors-having-global-exposure-like-it-oil-gas-icici-securities-122101200947_1.html</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>CAIiEP5WBMhr_vAMmT8knO0wdmwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEKC20lfPf2-af84FyyFQHowqGQgEKhAIACoHCAowsLXdCjCm3dEBMLPjpAM</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:29:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:50:00 GMT</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Apartments sales in 7 cities at 161k units in Jan-Sep; highest since 2015s  Business Standard</t>
+          <t>Avoid sectors having global exposure like IT, oil, gas: ICICI Securities  Business Standard</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3537,27 +3537,27 @@
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Jio most consistent, Airtel best 4G network for gaming in India: Reports - Business Standard</t>
+          <t>JoSAA 2022 round 5 allotment result declared; check details here - Business Standard</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/technology/jio-most-consistent-airtel-best-4g-network-for-gaming-in-india-report-122101100873_1.html</t>
+          <t>https://www.business-standard.com/article/education/josaa-2022-round-5-allotment-result-declared-check-details-here-122101201223_1.html</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>CAIiEHuwOYv4y7MeAMTnQ3Q_vg4qGQgEKhAIACoHCAowsLXdCjCm3dEBMPTgpAM</t>
+          <t>CAIiEIafKhczevy3yowmexfGLVgqGQgEKhAIACoHCAowsLXdCjCm3dEBMKS6swY</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 11:49:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:34:00 GMT</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Jio most consistent, Airtel best 4G network for gaming in India: Reports  Business Standard</t>
+          <t>JoSAA 2022 round 5 allotment result declared; check details here  Business Standard</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -3573,27 +3573,27 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Ministry proposes to decriminalise law on collection of statisticss - Business Standard</t>
+          <t>Red-hot defence stocks may have more legs to run, say analysts - Business Standard</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/ministry-proposes-to-decriminalise-law-on-collection-of-statistics-122101101154_1.html</t>
+          <t>https://www.business-standard.com/article/markets/red-hot-defence-stocks-may-have-more-legs-to-run-say-analysts-122101200998_1.html</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>CAIiEDwXzOE0STfSnq_b1Wo6XEYqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiECPO-sQhWS8wv6bThDvZmvwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:26:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:43:00 GMT</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Ministry proposes to decriminalise law on collection of statisticss  Business Standard</t>
+          <t>Red-hot defence stocks may have more legs to run, say analysts  Business Standard</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -3609,27 +3609,27 @@
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Masani re-elected as Prez of Asia Pacific Audit Bureaux of Certifications - Business Standard</t>
+          <t>Cabinet approves Rs 6,600 crore scheme PM-DevINE for North-Eastern states - Business Standard</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/masani-re-elected-as-prez-of-asia-pacific-audit-bureaux-of-certification-122101101147_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/cabinet-approves-rs-6-600-crore-scheme-pm-devine-for-north-eastern-states-122101201016_1.html</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>CAIiEP4kc9gpo6ztnS_8vacqhLAqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEKbdXPthslpUafLeRvA7rDkqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:23:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:16:00 GMT</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Masani re-elected as Prez of Asia Pacific Audit Bureaux of Certifications  Business Standard</t>
+          <t>Cabinet approves Rs 6,600 crore scheme PM-DevINE for North-Eastern states  Business Standard</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -3645,27 +3645,27 @@
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Elon Musk's affordable internet service Starlink debuts in Japan - Business Standard</t>
+          <t>Steel demand needs 9% CAGR to meet 160 kg/capita consumption target: Icra - Business Standard</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/elon-musk-s-affordable-internet-service-starlink-debuts-in-japan-122101100924_1.html</t>
+          <t>https://www.business-standard.com/article/markets/steel-demand-needs-9-cagr-to-meet-160-kg-capita-consumption-target-icra-122101201001_1.html</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>CAIiEPWEHZ4eDc4KrGO41TaQNeEqGQgEKhAIACoHCAowsLXdCjCm3dEBMKPkpAM</t>
+          <t>CAIiEMqjN_8W50ADfbWjB6evlFwqGQgEKhAIACoHCAowsLXdCjCm3dEBMLPjpAM</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 12:46:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:42:00 GMT</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Elon Musk's affordable internet service Starlink debuts in Japan  Business Standard</t>
+          <t>Steel demand needs 9% CAGR to meet 160 kg/capita consumption target: Icra  Business Standard</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -3681,27 +3681,27 @@
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Dont let exposure to mid and small-cap funds exceed 30%: Expertss - Business Standard</t>
+          <t>Govt amends Multi State Cooperative Societies Act to bring in transparency - Business Standard</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/pf/don-t-let-exposure-to-mid-small-cap-funds-exceed-30-experts-122101101142_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/cabinet-clears-amendments-to-multi-state-cooperative-societies-act-122101201091_1.html</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>CAIiEAqeTeQcpyZM67WHTSX4LXAqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEC4wsoq3LUzTjd2aKjRBecwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNPjpAM</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:22:00 GMT</t>
+          <t>Wed, 12 Oct 2022 14:46:00 GMT</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Dont let exposure to mid and small-cap funds exceed 30%: Expertss  Business Standard</t>
+          <t>Govt amends Multi State Cooperative Societies Act to bring in transparency  Business Standard</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -3717,27 +3717,27 @@
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Rising median loan rates lead to fall in affordability of homebuyerss - Business Standard</t>
+          <t>Reliance Retail, NBA sign contract to launch merchandise in India - Business Standard</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/rising-median-loan-rates-led-to-fall-in-affordability-of-homebuyers-by-2-122101101059_1.html</t>
+          <t>https://www.business-standard.com/article/companies/reliance-retail-nba-sign-contract-to-launch-merchandise-in-india-122101200966_1.html</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>CBMikAFodHRwczovL3d3dy5idXNpbmVzcy1zdGFuZGFyZC5jb20vYXJ0aWNsZS9jb21wYW5pZXMvcmlzaW5nLW1lZGlhbi1sb2FuLXJhdGVzLWxlZC10by1mYWxsLWluLWFmZm9yZGFiaWxpdHktb2YtaG9tZWJ1eWVycy1ieS0yLTEyMjEwMTEwMTA1OV8xLmh0bWzSAQA</t>
+          <t>CAIiEJQXzAXvX1g5Ift_0j7QBCAqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:16:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:29:00 GMT</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Rising median loan rates lead to fall in affordability of homebuyerss  Business Standard</t>
+          <t>Reliance Retail, NBA sign contract to launch merchandise in India  Business Standard</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -3753,27 +3753,27 @@
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Cisco launches India Webex infra, sees permanent shift to hybrid work models - Business Standard</t>
+          <t>Inter-regulatory push for the sandbox initiative: Check details here - Business Standard</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/companies/cisco-announces-dedicated-india-webex-infrastructure-with-data-centre-122101100998_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/inter-regulatory-push-for-sandbox-initiative-check-details-here-122101201126_1.html</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>CAIiEFlVBgDlepaT9CRPKE4QV3cqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
+          <t>CAIiEGwzcNMyv7eFvFKEdt8CwVAqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:50:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:24:00 GMT</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Cisco launches India Webex infra, sees permanent shift to hybrid work models  Business Standard</t>
+          <t>Inter-regulatory push for the sandbox initiative: Check details here  Business Standard</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -3789,27 +3789,27 @@
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr">
         <is>
-          <t>India up six places for reducing inequality, ranks 123 globally: Reports - Business Standard</t>
+          <t>EV solutions start-up Vecmocon raises $5.2 mn for business expansion - Business Standard</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/india-up-six-places-for-reducing-inequality-ranks-123-globally-report-122101100956_1.html</t>
+          <t>https://www.business-standard.com/article/companies/vecmocon-raises-5-2-mn-from-tiger-global-blume-ventures-and-others-122101200810_1.html</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>CAIiEEDS6a175Ih-LmyXHzgH9dQqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiECDZpfBKZqRl67gShZElxmsqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:47:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:19:00 GMT</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>India up six places for reducing inequality, ranks 123 globally: Reports  Business Standard</t>
+          <t>EV solutions start-up Vecmocon raises $5.2 mn for business expansion  Business Standard</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -3825,27 +3825,27 @@
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Govt offers 42 hydrocarbon blocks for exploration and development - Business Standard</t>
+          <t>Govt scraps sale of SAILs Bhadravathi plant on low bidder interest - Business Standard</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/economy-policy/centre-offers-42-oil-and-gas-blocks-for-exploration-development-122101101098_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/govt-scraps-sale-of-sail-s-bhadravathi-plant-on-low-bidder-interest-122101201130_1.html</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>CAIiEHUOa4UVvVFEK1HwDrVtHbUqGQgEKhAIACoHCAowsLXdCjCm3dEBMNPjpAM</t>
+          <t>CAIiEGo7Bt-dbvuc3HF0g1X34nIqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 14:03:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:21:00 GMT</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Govt offers 42 hydrocarbon blocks for exploration and development  Business Standard</t>
+          <t>Govt scraps sale of SAILs Bhadravathi plant on low bidder interest  Business Standard</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -3861,27 +3861,27 @@
       <c r="B96" t="inlineStr"/>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Railways passenger revenue in April-Oct 8 period up by 92% at Rs 33476 crs - Business Standard</t>
+          <t>Results preview: Strong operational show to drive Q2 for auto firms - Business Standard</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/railways-passenger-revenue-in-april-oct-8-period-up-by-92-at-rs-33-476-cr-122101101051_1.html</t>
+          <t>https://www.business-standard.com/article/companies/strong-operational-performance-to-drive-q2-earnings-at-auto-firms-122101201138_1.html</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>CAIiECsjDTIlkDP16jgDpETAfWIqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEHv-QSyNVpUEB3gxDBJC98UqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:55:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:27:00 GMT</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Railways passenger revenue in April-Oct 8 period up by 92% at Rs 33476 crs  Business Standard</t>
+          <t>Results preview: Strong operational show to drive Q2 for auto firms  Business Standard</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -3897,27 +3897,27 @@
       <c r="B97" t="inlineStr"/>
       <c r="C97" t="inlineStr">
         <is>
-          <t>US President Biden slams Russia for missile strikes across Ukraine - Business Standard</t>
+          <t>Ozonetel starts WhatsApp platform for firms customer communications - Business Standard</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/international/us-president-biden-slams-russia-for-missile-strikes-across-ukraine-122101100039_1.html</t>
+          <t>https://www.business-standard.com/article/companies/ozonetel-unveils-first-of-its-kind-contact-center-platform-on-whatsapp-122101200848_1.html</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>CAIiEGr8yKTXb8Gyh7G_eNbIQ_4qGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiEMc1PvbbZRkzPatsAq0O24AqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 03:36:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:22:00 GMT</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>US President Biden slams Russia for missile strikes across Ukraine  Business Standard</t>
+          <t>Ozonetel starts WhatsApp platform for firms customer communications  Business Standard</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -3933,27 +3933,27 @@
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Being in Jamkandorana is always special, says PM Modi during Gujarat rallys - Business Standard</t>
+          <t>Dish TV, 4 others settle non-disclosure of AGM voting results with Sebi - Business Standard</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/being-in-jamkandorana-is-always-special-says-pm-modi-during-gujarat-rally-122101100491_1.html</t>
+          <t>https://www.business-standard.com/article/companies/dish-tv-4-others-settle-non-disclosure-of-agm-voting-results-with-sebi-122101200999_1.html</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>CAIiEK5QZkSm72EAkJlo75JEbqgqGQgEKhAIACoHCAowsLXdCjCm3dEBMOPjpAM</t>
+          <t>CAIiEBT6LyLqjC7oXo-qqir0tfcqGQgEKhAIACoHCAowsLXdCjCm3dEBMIPjpAM</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 07:53:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:21:00 GMT</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Being in Jamkandorana is always special, says PM Modi during Gujarat rallys  Business Standard</t>
+          <t>Dish TV, 4 others settle non-disclosure of AGM voting results with Sebi  Business Standard</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -3969,27 +3969,27 @@
       <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr">
         <is>
-          <t>RBI allows SPDs to undertake all foreign exchange-related activitiess - Business Standard</t>
+          <t>172 workers at 56 airports found drunk on duty between Jan-July: DGCA - Business Standard</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/finance/rbi-allows-spds-to-undertake-all-foreign-exchange-related-activities-122101101053_1.html</t>
+          <t>https://www.business-standard.com/article/current-affairs/172-workers-at-56-airports-found-drunk-on-duty-between-jan-july-dgca-122101201147_1.html</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>CAIiEHJfuZsoCXvZRRIB5apMWZkqGQgEKhAIACoHCAowsLXdCjCm3dEBMMPjpAM</t>
+          <t>CAIiEBMmnMvxPvlNFQ4Ju0f5sYwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:59:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:14:00 GMT</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>RBI allows SPDs to undertake all foreign exchange-related activitiess  Business Standard</t>
+          <t>172 workers at 56 airports found drunk on duty between Jan-July: DGCA  Business Standard</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4005,27 +4005,27 @@
       <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr">
         <is>
-          <t>SC refuses to interfere with Bombay HC order granting bail to Anil Deshmukhs - Business Standard</t>
+          <t>Run-up to Budget: Monetary threshold for GST offences may rise to Rs 25 cr - Business Standard</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/current-affairs/sc-refuses-to-interfere-with-bombay-hc-order-granting-bail-to-anil-deshmukh-122101100935_1.html</t>
+          <t>https://www.business-standard.com/article/economy-policy/monetary-threshold-for-gst-related-offences-may-rise-to-rs-25-crore-122101201151_1.html</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>CAIiEF9GWNtJUjl3fhcuLPhq2GwqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
+          <t>CAIiENbBQxIlL_2llRCzraqfEVcqGQgEKhAIACoHCAowsLXdCjCm3dEBMNS-swY</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 12:48:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:14:00 GMT</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>SC refuses to interfere with Bombay HC order granting bail to Anil Deshmukhs  Business Standard</t>
+          <t>Run-up to Budget: Monetary threshold for GST offences may rise to Rs 25 cr  Business Standard</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4041,27 +4041,27 @@
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr">
         <is>
-          <t>MFI loans decline in June qtr; NPA situation improves, says reports - Business Standard</t>
+          <t>Half of top 500 stocks trading below their 200-DMA, shows data - Business Standard</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>https://www.business-standard.com/article/finance/mfi-loans-decline-in-june-qtr-npa-situation-improves-says-report-122101101072_1.html</t>
+          <t>https://www.business-standard.com/article/markets/over-half-of-top-500-stocks-dip-below-their-200-dma-shows-data-122101200929_1.html</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>CAIiEOPQZf-nHC-26bRqkdUt5wUqGQgEKhAIACoHCAowsLXdCjCm3dEBMMPjpAM</t>
+          <t>CAIiEJ-vVCzBalrf8ge2ORDRdtEqGQgEKhAIACoHCAowsLXdCjCm3dEBMOThpAM</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Tue, 11 Oct 2022 13:57:00 GMT</t>
+          <t>Wed, 12 Oct 2022 15:09:00 GMT</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>MFI loans decline in June qtr; NPA situation improves, says reports  Business Standard</t>
+          <t>Half of top 500 stocks trading below their 200-DMA, shows data  Business Standard</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">

</xml_diff>